<commit_message>
Se cambio a explorador edge y se comento la seccion de aviso de creacion de grupo de whatsapp
</commit_message>
<xml_diff>
--- a/modulo2.xlsx
+++ b/modulo2.xlsx
@@ -441,8 +441,8 @@
   </sheetPr>
   <dimension ref="A1:O500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView tabSelected="1" topLeftCell="F408" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B436" sqref="B436"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
@@ -28859,10 +28859,259 @@
         </is>
       </c>
     </row>
-    <row r="435"/>
-    <row r="436"/>
-    <row r="437"/>
-    <row r="438"/>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>2022-1</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>TU</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>IND-340</t>
+        </is>
+      </c>
+      <c r="D435" t="inlineStr">
+        <is>
+          <t>PROCESOS TERMICOS</t>
+        </is>
+      </c>
+      <c r="E435" t="inlineStr">
+        <is>
+          <t>VARIABLE</t>
+        </is>
+      </c>
+      <c r="F435" t="inlineStr">
+        <is>
+          <t>HORARIO VARIABLE</t>
+        </is>
+      </c>
+      <c r="G435" t="inlineStr">
+        <is>
+          <t>TUTORIA-PRESENCIAL</t>
+        </is>
+      </c>
+      <c r="H435" t="inlineStr">
+        <is>
+          <t>ROJAS</t>
+        </is>
+      </c>
+      <c r="I435" t="inlineStr">
+        <is>
+          <t>GALARZA</t>
+        </is>
+      </c>
+      <c r="J435" t="inlineStr">
+        <is>
+          <t>GEORGINA</t>
+        </is>
+      </c>
+      <c r="K435" t="inlineStr">
+        <is>
+          <t>INDUSTRIAL</t>
+        </is>
+      </c>
+      <c r="L435" t="inlineStr">
+        <is>
+          <t>https://chat.whatsapp.com/FT24u5PZ4SfB4ML8V9dyTN</t>
+        </is>
+      </c>
+      <c r="M435" t="inlineStr">
+        <is>
+          <t>PROCESOS.TERMICOS_TU</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>2022-1</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>COM-160</t>
+        </is>
+      </c>
+      <c r="D436" t="inlineStr">
+        <is>
+          <t>TOPICOS (INDUSTRIAL)</t>
+        </is>
+      </c>
+      <c r="E436" t="inlineStr">
+        <is>
+          <t>19:15-21:45</t>
+        </is>
+      </c>
+      <c r="F436" t="inlineStr">
+        <is>
+          <t>NOCHE</t>
+        </is>
+      </c>
+      <c r="G436" t="inlineStr">
+        <is>
+          <t>PRESENCIAL</t>
+        </is>
+      </c>
+      <c r="K436" t="inlineStr">
+        <is>
+          <t>INDUSTRIAL</t>
+        </is>
+      </c>
+      <c r="L436" t="inlineStr">
+        <is>
+          <t>https://chat.whatsapp.com/Lt1NTnPojAkFuyucW3pn9R</t>
+        </is>
+      </c>
+      <c r="M436" t="inlineStr">
+        <is>
+          <t>TOPICOS.INDUSTRIAL_B</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>2022-1</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>FAU-307</t>
+        </is>
+      </c>
+      <c r="D437" t="inlineStr">
+        <is>
+          <t>TALLER DE GRADUACION</t>
+        </is>
+      </c>
+      <c r="E437" t="inlineStr">
+        <is>
+          <t>19:30-21:30</t>
+        </is>
+      </c>
+      <c r="F437" t="inlineStr">
+        <is>
+          <t>P.T. NOCHE M-J</t>
+        </is>
+      </c>
+      <c r="G437" t="inlineStr">
+        <is>
+          <t>SEMI-PRESENCIAL</t>
+        </is>
+      </c>
+      <c r="H437" t="inlineStr">
+        <is>
+          <t>CESPEDES</t>
+        </is>
+      </c>
+      <c r="I437" t="inlineStr">
+        <is>
+          <t>SANCHEZ</t>
+        </is>
+      </c>
+      <c r="J437" t="inlineStr">
+        <is>
+          <t>CARMEN ROSA</t>
+        </is>
+      </c>
+      <c r="K437" t="inlineStr">
+        <is>
+          <t>MARKETING</t>
+        </is>
+      </c>
+      <c r="L437" t="inlineStr">
+        <is>
+          <t>https://chat.whatsapp.com/ECkSSSoHgDN2nmezoVxw1g</t>
+        </is>
+      </c>
+      <c r="M437" t="inlineStr">
+        <is>
+          <t>TALLER.GRADUACION_X</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>2022-1</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>PRO-730</t>
+        </is>
+      </c>
+      <c r="D438" t="inlineStr">
+        <is>
+          <t>SEMINARIO DE GRADO</t>
+        </is>
+      </c>
+      <c r="E438" t="inlineStr">
+        <is>
+          <t>07:15-10:00</t>
+        </is>
+      </c>
+      <c r="F438" t="inlineStr">
+        <is>
+          <t>MAÑANA</t>
+        </is>
+      </c>
+      <c r="G438" t="inlineStr">
+        <is>
+          <t>PRESENCIAL</t>
+        </is>
+      </c>
+      <c r="H438" t="inlineStr">
+        <is>
+          <t>PEDRAZA</t>
+        </is>
+      </c>
+      <c r="I438" t="inlineStr">
+        <is>
+          <t>RIVERO</t>
+        </is>
+      </c>
+      <c r="J438" t="inlineStr">
+        <is>
+          <t>VERONICA</t>
+        </is>
+      </c>
+      <c r="K438" t="inlineStr">
+        <is>
+          <t>MARKETING</t>
+        </is>
+      </c>
+      <c r="L438" t="inlineStr">
+        <is>
+          <t>https://chat.whatsapp.com/G0N3UEsmiKjAUnGekxW0sk</t>
+        </is>
+      </c>
+      <c r="M438" t="inlineStr">
+        <is>
+          <t>SEMINARIO.GRADO_A</t>
+        </is>
+      </c>
+    </row>
     <row r="439"/>
     <row r="440"/>
     <row r="441"/>

</xml_diff>